<commit_message>
finished to rename Cube in VS2022 through the live connection SSAS
</commit_message>
<xml_diff>
--- a/BISolutionWorksheets.xlsx
+++ b/BISolutionWorksheets.xlsx
@@ -636,9 +636,6 @@
     <t>DWNorthwindOrders.dbo.FactOrders.ShippedDateKey</t>
   </si>
   <si>
-    <t>CubeOrders</t>
-  </si>
-  <si>
     <t>Provides order information</t>
   </si>
   <si>
@@ -1558,6 +1555,9 @@
   </si>
   <si>
     <t>Calendar-Year</t>
+  </si>
+  <si>
+    <t>CubeNorthwindOrders</t>
   </si>
 </sst>
 </file>
@@ -3623,7 +3623,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="51" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B1" s="51"/>
       <c r="C1" s="52"/>
@@ -3645,163 +3645,163 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2" t="s">
         <v>304</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>305</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>306</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>307</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>308</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>309</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>310</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>311</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>312</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>313</v>
-      </c>
-      <c r="K2" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>314</v>
+      </c>
+      <c r="B3" t="s">
         <v>315</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>316</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>317</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>318</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>319</v>
       </c>
-      <c r="F3" t="s">
-        <v>320</v>
-      </c>
       <c r="G3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H3">
         <v>12209</v>
       </c>
       <c r="I3" t="s">
+        <v>321</v>
+      </c>
+      <c r="J3" t="s">
         <v>322</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>323</v>
-      </c>
-      <c r="K3" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>324</v>
+      </c>
+      <c r="B4" t="s">
         <v>325</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>326</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>327</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>328</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>329</v>
       </c>
-      <c r="F4" t="s">
-        <v>330</v>
-      </c>
       <c r="G4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H4">
         <v>5021</v>
       </c>
       <c r="I4" t="s">
+        <v>330</v>
+      </c>
+      <c r="J4" t="s">
         <v>331</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>332</v>
-      </c>
-      <c r="K4" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>333</v>
+      </c>
+      <c r="B6" t="s">
         <v>334</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>335</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>336</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>337</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>338</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>339</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
+        <v>307</v>
+      </c>
+      <c r="I6" t="s">
+        <v>308</v>
+      </c>
+      <c r="J6" t="s">
+        <v>309</v>
+      </c>
+      <c r="K6" t="s">
+        <v>310</v>
+      </c>
+      <c r="L6" t="s">
+        <v>311</v>
+      </c>
+      <c r="M6" t="s">
         <v>340</v>
       </c>
-      <c r="H6" t="s">
-        <v>308</v>
-      </c>
-      <c r="I6" t="s">
-        <v>309</v>
-      </c>
-      <c r="J6" t="s">
-        <v>310</v>
-      </c>
-      <c r="K6" t="s">
-        <v>311</v>
-      </c>
-      <c r="L6" t="s">
-        <v>312</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>341</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>342</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>343</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>344</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>345</v>
-      </c>
-      <c r="R6" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -3809,16 +3809,16 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>346</v>
+      </c>
+      <c r="C7" t="s">
         <v>347</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>317</v>
+      </c>
+      <c r="E7" t="s">
         <v>348</v>
-      </c>
-      <c r="D7" t="s">
-        <v>318</v>
-      </c>
-      <c r="E7" t="s">
-        <v>349</v>
       </c>
       <c r="F7" s="53">
         <v>17875</v>
@@ -3827,37 +3827,37 @@
         <v>33725</v>
       </c>
       <c r="H7" t="s">
+        <v>349</v>
+      </c>
+      <c r="I7" t="s">
         <v>350</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>351</v>
-      </c>
-      <c r="J7" t="s">
-        <v>352</v>
       </c>
       <c r="K7">
         <v>98122</v>
       </c>
       <c r="L7" t="s">
+        <v>352</v>
+      </c>
+      <c r="M7" t="s">
         <v>353</v>
-      </c>
-      <c r="M7" t="s">
-        <v>354</v>
       </c>
       <c r="N7">
         <v>5467</v>
       </c>
       <c r="O7" t="s">
+        <v>354</v>
+      </c>
+      <c r="P7" t="s">
         <v>355</v>
-      </c>
-      <c r="P7" t="s">
-        <v>356</v>
       </c>
       <c r="Q7">
         <v>2</v>
       </c>
       <c r="R7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -3865,16 +3865,16 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
+        <v>357</v>
+      </c>
+      <c r="C8" t="s">
         <v>358</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>359</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>360</v>
-      </c>
-      <c r="E8" t="s">
-        <v>361</v>
       </c>
       <c r="F8" s="53">
         <v>19043</v>
@@ -3883,81 +3883,81 @@
         <v>33830</v>
       </c>
       <c r="H8" t="s">
+        <v>361</v>
+      </c>
+      <c r="I8" t="s">
         <v>362</v>
       </c>
-      <c r="I8" t="s">
-        <v>363</v>
-      </c>
       <c r="J8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K8">
         <v>98401</v>
       </c>
       <c r="L8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="N8">
         <v>3457</v>
       </c>
       <c r="O8" t="s">
+        <v>354</v>
+      </c>
+      <c r="P8" t="s">
         <v>355</v>
       </c>
-      <c r="P8" t="s">
-        <v>356</v>
-      </c>
       <c r="Q8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="R8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>365</v>
+      </c>
+      <c r="B10" t="s">
+        <v>303</v>
+      </c>
+      <c r="C10" t="s">
+        <v>333</v>
+      </c>
+      <c r="D10" t="s">
         <v>366</v>
       </c>
-      <c r="B10" t="s">
-        <v>304</v>
-      </c>
-      <c r="C10" t="s">
-        <v>334</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>367</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>368</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>369</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>370</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>371</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>372</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>373</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>374</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>375</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>376</v>
-      </c>
-      <c r="N10" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -3965,7 +3965,7 @@
         <v>10248</v>
       </c>
       <c r="B11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -3986,22 +3986,22 @@
         <v>32.380000000000003</v>
       </c>
       <c r="I11" t="s">
+        <v>378</v>
+      </c>
+      <c r="J11" t="s">
         <v>379</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>380</v>
       </c>
-      <c r="K11" t="s">
-        <v>381</v>
-      </c>
       <c r="L11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="M11">
         <v>51100</v>
       </c>
       <c r="N11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -4009,7 +4009,7 @@
         <v>10249</v>
       </c>
       <c r="B12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C12">
         <v>6</v>
@@ -4030,22 +4030,22 @@
         <v>11.61</v>
       </c>
       <c r="I12" t="s">
+        <v>383</v>
+      </c>
+      <c r="J12" t="s">
         <v>384</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>385</v>
       </c>
-      <c r="K12" t="s">
-        <v>386</v>
-      </c>
       <c r="L12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="M12">
         <v>44087</v>
       </c>
       <c r="N12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -4055,19 +4055,19 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B14" t="s">
+        <v>386</v>
+      </c>
+      <c r="C14" t="s">
         <v>387</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" s="54" t="s">
         <v>388</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="E14" s="54" t="s">
         <v>389</v>
-      </c>
-      <c r="E14" s="54" t="s">
-        <v>390</v>
       </c>
       <c r="F14" s="54"/>
     </row>
@@ -4114,34 +4114,34 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>386</v>
+      </c>
+      <c r="B18" t="s">
+        <v>390</v>
+      </c>
+      <c r="C18" t="s">
+        <v>391</v>
+      </c>
+      <c r="D18" s="54" t="s">
+        <v>392</v>
+      </c>
+      <c r="E18" s="54" t="s">
+        <v>393</v>
+      </c>
+      <c r="F18" s="54" t="s">
         <v>387</v>
       </c>
-      <c r="B18" t="s">
-        <v>391</v>
-      </c>
-      <c r="C18" t="s">
-        <v>392</v>
-      </c>
-      <c r="D18" s="54" t="s">
-        <v>393</v>
-      </c>
-      <c r="E18" s="54" t="s">
+      <c r="G18" t="s">
         <v>394</v>
       </c>
-      <c r="F18" s="54" t="s">
-        <v>388</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>395</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>396</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>397</v>
-      </c>
-      <c r="J18" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -4149,7 +4149,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -4158,7 +4158,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="54" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F19">
         <v>18</v>
@@ -4181,7 +4181,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -4190,7 +4190,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="54" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F20">
         <v>19</v>
@@ -4215,16 +4215,16 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B22" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E22" s="54"/>
       <c r="F22" s="54"/>
@@ -4234,13 +4234,13 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
+        <v>404</v>
+      </c>
+      <c r="C23" t="s">
         <v>405</v>
       </c>
-      <c r="C23" t="s">
-        <v>406</v>
-      </c>
       <c r="D23" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E23" s="54"/>
       <c r="F23" s="54"/>
@@ -4250,13 +4250,13 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
+        <v>406</v>
+      </c>
+      <c r="C24" t="s">
         <v>407</v>
       </c>
-      <c r="C24" t="s">
-        <v>408</v>
-      </c>
       <c r="D24" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E24" s="54"/>
       <c r="F24" s="54"/>
@@ -4268,7 +4268,7 @@
     </row>
     <row r="26" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="51" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B26" s="51"/>
       <c r="C26" s="52"/>
@@ -4281,1887 +4281,1887 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>409</v>
+      </c>
+      <c r="B27" t="s">
         <v>410</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>411</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>412</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>413</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>414</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>415</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>416</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>417</v>
-      </c>
-      <c r="I27" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B28" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
       </c>
       <c r="D28" t="s">
+        <v>419</v>
+      </c>
+      <c r="E28" t="s">
         <v>420</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>421</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
+        <v>320</v>
+      </c>
+      <c r="H28" t="s">
+        <v>320</v>
+      </c>
+      <c r="I28" t="s">
         <v>422</v>
-      </c>
-      <c r="G28" t="s">
-        <v>321</v>
-      </c>
-      <c r="H28" t="s">
-        <v>321</v>
-      </c>
-      <c r="I28" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B29" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C29" t="s">
         <v>174</v>
       </c>
       <c r="D29" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E29" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F29" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G29" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H29" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I29" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B30" t="s">
         <v>2</v>
       </c>
       <c r="C30" t="s">
+        <v>424</v>
+      </c>
+      <c r="D30" t="s">
+        <v>320</v>
+      </c>
+      <c r="E30" t="s">
+        <v>320</v>
+      </c>
+      <c r="F30" t="s">
         <v>425</v>
       </c>
-      <c r="D30" t="s">
-        <v>321</v>
-      </c>
-      <c r="E30" t="s">
-        <v>321</v>
-      </c>
-      <c r="F30" t="s">
-        <v>426</v>
-      </c>
       <c r="G30" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H30" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I30" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B31" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C31" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D31" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E31" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F31" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G31" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H31" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I31" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B32" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C32" t="s">
         <v>154</v>
       </c>
       <c r="D32" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E32" t="s">
+        <v>420</v>
+      </c>
+      <c r="F32" t="s">
         <v>421</v>
       </c>
-      <c r="F32" t="s">
-        <v>422</v>
-      </c>
       <c r="G32" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H32" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I32" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B33" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C33" t="s">
         <v>170</v>
       </c>
       <c r="D33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F33" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I33" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B34" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C34" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D34" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E34" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F34" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G34" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H34" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I34" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B35" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C35" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D35" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E35" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F35" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G35" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H35" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I35" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B36" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C36" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D36" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E36" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G36" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H36" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I36" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B37" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C37" t="s">
         <v>174</v>
       </c>
       <c r="D37" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E37" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F37" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G37" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H37" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I37" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B38" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C38" t="s">
         <v>174</v>
       </c>
       <c r="D38" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E38" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F38" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G38" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H38" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I38" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B39" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C39" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D39" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E39" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F39" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G39" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H39" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I39" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B40" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C40" t="s">
         <v>174</v>
       </c>
       <c r="D40" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E40" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F40" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G40" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H40" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I40" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B41" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C41" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D41" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E41" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F41" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G41" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H41" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I41" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B42" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C42" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D42" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E42" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F42" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G42" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H42" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I42" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C43" t="s">
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E43" t="s">
+        <v>420</v>
+      </c>
+      <c r="F43" t="s">
         <v>421</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
+        <v>320</v>
+      </c>
+      <c r="H43" t="s">
+        <v>320</v>
+      </c>
+      <c r="I43" t="s">
         <v>422</v>
-      </c>
-      <c r="G43" t="s">
-        <v>321</v>
-      </c>
-      <c r="H43" t="s">
-        <v>321</v>
-      </c>
-      <c r="I43" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B44" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C44" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D44" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E44" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F44" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G44" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H44" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I44" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B45" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C45" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D45" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E45" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F45" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G45" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H45" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I45" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B46" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C46" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D46" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E46" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F46" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G46" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H46" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I46" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B47" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C47" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D47" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E47" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F47" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G47" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H47" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I47" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B48" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C48" t="s">
         <v>93</v>
       </c>
       <c r="D48" t="s">
+        <v>436</v>
+      </c>
+      <c r="E48" t="s">
         <v>437</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
+        <v>425</v>
+      </c>
+      <c r="G48" t="s">
         <v>438</v>
       </c>
-      <c r="F48" t="s">
-        <v>426</v>
-      </c>
-      <c r="G48" t="s">
-        <v>439</v>
-      </c>
       <c r="H48" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I48" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B49" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C49" t="s">
         <v>93</v>
       </c>
       <c r="D49" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E49" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F49" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G49" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H49" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I49" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B50" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C50" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D50" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E50" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F50" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G50" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H50" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I50" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B51" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C51" t="s">
         <v>174</v>
       </c>
       <c r="D51" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E51" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F51" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G51" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H51" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I51" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B52" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C52" t="s">
         <v>174</v>
       </c>
       <c r="D52" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E52" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F52" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G52" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H52" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I52" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B53" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C53" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D53" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E53" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F53" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G53" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H53" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I53" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B54" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C54" t="s">
         <v>174</v>
       </c>
       <c r="D54" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E54" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F54" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G54" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H54" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I54" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B55" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C55" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D55" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E55" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F55" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G55" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H55" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I55" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B56" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C56" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D56" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E56" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F56" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G56" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H56" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I56" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B57" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C57" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D57" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E57" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F57" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G57" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H57" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I57" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B58" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C58" t="s">
+        <v>424</v>
+      </c>
+      <c r="D58" t="s">
+        <v>320</v>
+      </c>
+      <c r="E58" t="s">
+        <v>320</v>
+      </c>
+      <c r="F58" t="s">
         <v>425</v>
       </c>
-      <c r="D58" t="s">
-        <v>321</v>
-      </c>
-      <c r="E58" t="s">
-        <v>321</v>
-      </c>
-      <c r="F58" t="s">
-        <v>426</v>
-      </c>
       <c r="G58" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H58" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I58" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B59" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C59" t="s">
         <v>9</v>
       </c>
       <c r="D59" t="s">
+        <v>440</v>
+      </c>
+      <c r="E59" t="s">
         <v>441</v>
       </c>
-      <c r="E59" t="s">
-        <v>442</v>
-      </c>
       <c r="F59" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G59" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H59" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I59" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B60" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C60" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D60" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E60" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F60" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G60" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H60" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I60" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B61" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C61" t="s">
         <v>9</v>
       </c>
       <c r="D61" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E61" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F61" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G61" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H61" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I61" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B62" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C62" t="s">
         <v>9</v>
       </c>
       <c r="D62" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E62" t="s">
+        <v>420</v>
+      </c>
+      <c r="F62" t="s">
         <v>421</v>
       </c>
-      <c r="F62" t="s">
-        <v>422</v>
-      </c>
       <c r="G62" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H62" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I62" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B63" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C63" t="s">
         <v>9</v>
       </c>
       <c r="D63" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E63" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F63" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G63" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H63" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I63" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B64" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C64" t="s">
         <v>9</v>
       </c>
       <c r="D64" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E64" t="s">
+        <v>420</v>
+      </c>
+      <c r="F64" t="s">
         <v>421</v>
       </c>
-      <c r="F64" t="s">
-        <v>422</v>
-      </c>
       <c r="G64" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H64" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I64" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B65" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C65" t="s">
         <v>106</v>
       </c>
       <c r="D65" t="s">
+        <v>447</v>
+      </c>
+      <c r="E65" t="s">
+        <v>437</v>
+      </c>
+      <c r="F65" t="s">
+        <v>421</v>
+      </c>
+      <c r="G65" t="s">
         <v>448</v>
       </c>
-      <c r="E65" t="s">
-        <v>438</v>
-      </c>
-      <c r="F65" t="s">
-        <v>422</v>
-      </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>449</v>
       </c>
-      <c r="H65" t="s">
-        <v>450</v>
-      </c>
       <c r="I65" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B66" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C66" t="s">
         <v>129</v>
       </c>
       <c r="D66" t="s">
+        <v>450</v>
+      </c>
+      <c r="E66" t="s">
+        <v>437</v>
+      </c>
+      <c r="F66" t="s">
+        <v>421</v>
+      </c>
+      <c r="G66" t="s">
         <v>451</v>
       </c>
-      <c r="E66" t="s">
-        <v>438</v>
-      </c>
-      <c r="F66" t="s">
-        <v>422</v>
-      </c>
-      <c r="G66" t="s">
+      <c r="H66" t="s">
         <v>452</v>
       </c>
-      <c r="H66" t="s">
-        <v>453</v>
-      </c>
       <c r="I66" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B67" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C67" t="s">
+        <v>453</v>
+      </c>
+      <c r="D67" t="s">
         <v>454</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
+        <v>437</v>
+      </c>
+      <c r="F67" t="s">
+        <v>421</v>
+      </c>
+      <c r="G67" t="s">
         <v>455</v>
       </c>
-      <c r="E67" t="s">
-        <v>438</v>
-      </c>
-      <c r="F67" t="s">
-        <v>422</v>
-      </c>
-      <c r="G67" t="s">
-        <v>456</v>
-      </c>
       <c r="H67" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I67" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B68" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C68" t="s">
         <v>9</v>
       </c>
       <c r="D68" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E68" t="s">
+        <v>420</v>
+      </c>
+      <c r="F68" t="s">
         <v>421</v>
       </c>
-      <c r="F68" t="s">
+      <c r="G68" t="s">
+        <v>320</v>
+      </c>
+      <c r="H68" t="s">
+        <v>320</v>
+      </c>
+      <c r="I68" t="s">
         <v>422</v>
-      </c>
-      <c r="G68" t="s">
-        <v>321</v>
-      </c>
-      <c r="H68" t="s">
-        <v>321</v>
-      </c>
-      <c r="I68" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B69" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C69" t="s">
         <v>154</v>
       </c>
       <c r="D69" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E69" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F69" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G69" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H69" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I69" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B70" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C70" t="s">
         <v>9</v>
       </c>
       <c r="D70" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E70" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F70" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G70" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H70" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I70" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B71" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C71" t="s">
         <v>93</v>
       </c>
       <c r="D71" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E71" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F71" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G71" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H71" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I71" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B72" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C72" t="s">
         <v>93</v>
       </c>
       <c r="D72" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E72" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F72" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G72" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H72" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I72" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B73" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C73" t="s">
         <v>93</v>
       </c>
       <c r="D73" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E73" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F73" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G73" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H73" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I73" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B74" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C74" t="s">
         <v>9</v>
       </c>
       <c r="D74" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E74" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F74" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G74" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H74" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I74" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B75" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C75" t="s">
         <v>106</v>
       </c>
       <c r="D75" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E75" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F75" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G75" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H75" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I75" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B76" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C76" t="s">
         <v>170</v>
       </c>
       <c r="D76" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E76" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F76" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G76" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H76" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I76" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B77" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C77" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D77" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E77" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F77" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G77" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H77" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I77" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B78" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C78" t="s">
         <v>174</v>
       </c>
       <c r="D78" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E78" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F78" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G78" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H78" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I78" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B79" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C79" t="s">
         <v>174</v>
       </c>
       <c r="D79" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E79" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F79" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G79" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H79" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I79" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B80" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C80" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D80" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E80" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F80" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G80" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H80" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I80" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B81" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C81" t="s">
         <v>174</v>
       </c>
       <c r="D81" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E81" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F81" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G81" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H81" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I81" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B82" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C82" t="s">
         <v>9</v>
       </c>
       <c r="D82" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E82" t="s">
+        <v>420</v>
+      </c>
+      <c r="F82" t="s">
         <v>421</v>
       </c>
-      <c r="F82" t="s">
+      <c r="G82" t="s">
+        <v>320</v>
+      </c>
+      <c r="H82" t="s">
+        <v>320</v>
+      </c>
+      <c r="I82" t="s">
         <v>422</v>
-      </c>
-      <c r="G82" t="s">
-        <v>321</v>
-      </c>
-      <c r="H82" t="s">
-        <v>321</v>
-      </c>
-      <c r="I82" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B83" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C83" t="s">
         <v>170</v>
       </c>
       <c r="D83" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E83" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F83" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G83" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H83" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I83" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B84" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C84" t="s">
         <v>9</v>
       </c>
       <c r="D84" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E84" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F84" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G84" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H84" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I84" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B85" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C85" t="s">
         <v>9</v>
       </c>
       <c r="D85" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E85" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F85" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G85" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H85" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I85" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B86" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C86" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D86" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E86" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F86" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G86" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H86" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I86" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B87" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C87" t="s">
         <v>106</v>
       </c>
       <c r="D87" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E87" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F87" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G87" t="s">
+        <v>448</v>
+      </c>
+      <c r="H87" t="s">
         <v>449</v>
       </c>
-      <c r="H87" t="s">
-        <v>450</v>
-      </c>
       <c r="I87" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B88" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C88" t="s">
         <v>129</v>
       </c>
       <c r="D88" t="s">
+        <v>466</v>
+      </c>
+      <c r="E88" t="s">
+        <v>437</v>
+      </c>
+      <c r="F88" t="s">
+        <v>425</v>
+      </c>
+      <c r="G88" t="s">
         <v>467</v>
       </c>
-      <c r="E88" t="s">
-        <v>438</v>
-      </c>
-      <c r="F88" t="s">
-        <v>426</v>
-      </c>
-      <c r="G88" t="s">
-        <v>468</v>
-      </c>
       <c r="H88" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I88" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B89" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C89" t="s">
         <v>129</v>
       </c>
       <c r="D89" t="s">
+        <v>468</v>
+      </c>
+      <c r="E89" t="s">
+        <v>437</v>
+      </c>
+      <c r="F89" t="s">
+        <v>425</v>
+      </c>
+      <c r="G89" t="s">
         <v>469</v>
       </c>
-      <c r="E89" t="s">
-        <v>438</v>
-      </c>
-      <c r="F89" t="s">
-        <v>426</v>
-      </c>
-      <c r="G89" t="s">
-        <v>470</v>
-      </c>
       <c r="H89" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I89" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B90" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C90" t="s">
         <v>129</v>
       </c>
       <c r="D90" t="s">
+        <v>470</v>
+      </c>
+      <c r="E90" t="s">
+        <v>437</v>
+      </c>
+      <c r="F90" t="s">
+        <v>425</v>
+      </c>
+      <c r="G90" t="s">
         <v>471</v>
       </c>
-      <c r="E90" t="s">
-        <v>438</v>
-      </c>
-      <c r="F90" t="s">
-        <v>426</v>
-      </c>
-      <c r="G90" t="s">
-        <v>472</v>
-      </c>
       <c r="H90" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I90" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B91" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C91" t="s">
         <v>187</v>
       </c>
       <c r="D91" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E91" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F91" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G91" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H91" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I91" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -6217,7 +6217,7 @@
         <v>8</v>
       </c>
       <c r="F4" s="47" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -6273,7 +6273,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="48" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -6293,7 +6293,7 @@
         <v>9</v>
       </c>
       <c r="F8" s="48" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -6313,7 +6313,7 @@
         <v>9</v>
       </c>
       <c r="F9" s="48" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -6333,7 +6333,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="48" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -6353,7 +6353,7 @@
         <v>9</v>
       </c>
       <c r="F11" s="48" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -6373,7 +6373,7 @@
         <v>9</v>
       </c>
       <c r="F12" s="48" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -6393,7 +6393,7 @@
         <v>9</v>
       </c>
       <c r="F13" s="48" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -6413,7 +6413,7 @@
         <v>9</v>
       </c>
       <c r="F14" s="49" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -6433,7 +6433,7 @@
         <v>110</v>
       </c>
       <c r="F15" s="49" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -6471,7 +6471,7 @@
         <v>9</v>
       </c>
       <c r="F17" s="49" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -6491,7 +6491,7 @@
         <v>154</v>
       </c>
       <c r="F18" s="49" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -6511,7 +6511,7 @@
         <v>130</v>
       </c>
       <c r="F19" s="49" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -6531,7 +6531,7 @@
         <v>107</v>
       </c>
       <c r="F20" s="49" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -6551,7 +6551,7 @@
         <v>107</v>
       </c>
       <c r="F21" s="49" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -6571,7 +6571,7 @@
         <v>107</v>
       </c>
       <c r="F22" s="49" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -6609,7 +6609,7 @@
         <v>9</v>
       </c>
       <c r="F24" s="49" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -6629,7 +6629,7 @@
         <v>9</v>
       </c>
       <c r="F25" s="49" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -6649,7 +6649,7 @@
         <v>130</v>
       </c>
       <c r="F26" s="49" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -6669,7 +6669,7 @@
         <v>130</v>
       </c>
       <c r="F27" s="49" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -6689,7 +6689,7 @@
         <v>110</v>
       </c>
       <c r="F28" s="49" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -6709,7 +6709,7 @@
         <v>197</v>
       </c>
       <c r="F29" s="49" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -6747,7 +6747,7 @@
         <v>9</v>
       </c>
       <c r="F31" s="49" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -6767,7 +6767,7 @@
         <v>9</v>
       </c>
       <c r="F32" s="49" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -6787,7 +6787,7 @@
         <v>130</v>
       </c>
       <c r="F33" s="49" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -6807,7 +6807,7 @@
         <v>9</v>
       </c>
       <c r="F34" s="49" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -6827,7 +6827,7 @@
         <v>9</v>
       </c>
       <c r="F35" s="49" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -6865,7 +6865,7 @@
         <v>9</v>
       </c>
       <c r="F37" s="50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -6885,7 +6885,7 @@
         <v>93</v>
       </c>
       <c r="F38" s="50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -6905,7 +6905,7 @@
         <v>107</v>
       </c>
       <c r="F39" s="50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -6925,7 +6925,7 @@
         <v>9</v>
       </c>
       <c r="F40" s="50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -6945,7 +6945,7 @@
         <v>107</v>
       </c>
       <c r="F41" s="50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -6965,7 +6965,7 @@
         <v>9</v>
       </c>
       <c r="F42" s="50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -6985,7 +6985,7 @@
         <v>107</v>
       </c>
       <c r="F43" s="50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -7005,7 +7005,7 @@
         <v>9</v>
       </c>
       <c r="F44" s="50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -7025,7 +7025,7 @@
         <v>107</v>
       </c>
       <c r="F45" s="50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -7097,29 +7097,29 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="60" t="s">
+        <v>289</v>
+      </c>
+      <c r="B4" s="60" t="s">
         <v>290</v>
       </c>
-      <c r="B4" s="60" t="s">
-        <v>291</v>
-      </c>
       <c r="C4" s="60" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D4" s="61"/>
       <c r="E4" s="61"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="60" t="s">
+        <v>298</v>
+      </c>
+      <c r="B5" s="60" t="s">
         <v>299</v>
       </c>
-      <c r="B5" s="60" t="s">
-        <v>300</v>
-      </c>
       <c r="C5" s="60" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D5" s="61" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E5" s="61"/>
     </row>
@@ -7128,90 +7128,90 @@
         <v>132</v>
       </c>
       <c r="B6" s="60" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C6" s="60" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D6" s="61"/>
       <c r="E6" s="61" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="B7" s="62" t="s">
         <v>292</v>
       </c>
-      <c r="B7" s="62" t="s">
-        <v>293</v>
-      </c>
       <c r="C7" s="62" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D7" s="63"/>
       <c r="E7" s="63"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="64" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C8" s="64" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D8" s="65"/>
       <c r="E8" s="65"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="64" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B9" s="64" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D9" s="65"/>
       <c r="E9" s="65"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="62" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B10" s="62" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C10" s="62" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D10" s="63"/>
       <c r="E10" s="63"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="42" t="s">
+        <v>274</v>
+      </c>
+      <c r="B11" s="42" t="s">
         <v>275</v>
       </c>
-      <c r="B11" s="42" t="s">
-        <v>276</v>
-      </c>
       <c r="C11" s="42" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D11" s="42"/>
       <c r="E11" s="42"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="66" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B12" s="66" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C12" s="66" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D12" s="66" t="s">
         <v>161</v>
@@ -7220,13 +7220,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="66" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B13" s="66" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C13" s="66" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D13" s="66"/>
       <c r="E13" s="66" t="s">
@@ -7235,39 +7235,39 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="64" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B14" s="64" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C14" s="64" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D14" s="65"/>
       <c r="E14" s="65"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="42" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B15" s="42" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D15" s="65"/>
       <c r="E15" s="65"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="66" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B16" s="66" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C16" s="66" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D16" s="66" t="s">
         <v>164</v>
@@ -7276,13 +7276,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="66" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B17" s="66" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C17" s="66" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D17" s="67"/>
       <c r="E17" s="66" t="s">
@@ -7291,78 +7291,78 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="42" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B18" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C18" s="42" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D18" s="65"/>
       <c r="E18" s="65"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="42" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D19" s="65"/>
       <c r="E19" s="65"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="68" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B20" s="68" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C20" s="68" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D20" s="63"/>
       <c r="E20" s="63"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="42" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D21" s="65"/>
       <c r="E21" s="65"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="68" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B22" s="68" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C22" s="68" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D22" s="63"/>
       <c r="E22" s="63"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="42" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B23" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D23" s="65"/>
       <c r="E23" s="65"/>
@@ -7380,8 +7380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7403,10 +7403,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="44" t="s">
+        <v>502</v>
+      </c>
+      <c r="C3" s="44" t="s">
         <v>503</v>
-      </c>
-      <c r="C3" s="44" t="s">
-        <v>504</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>2</v>
@@ -7417,423 +7417,423 @@
         <v>132</v>
       </c>
       <c r="B4" s="45" t="s">
+        <v>492</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>504</v>
+      </c>
+      <c r="D4" s="45" t="s">
         <v>493</v>
-      </c>
-      <c r="C4" s="45" t="s">
-        <v>505</v>
-      </c>
-      <c r="D4" s="45" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="45" t="s">
+        <v>494</v>
+      </c>
+      <c r="B5" s="45" t="s">
         <v>495</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="C5" s="45" t="s">
+        <v>504</v>
+      </c>
+      <c r="D5" s="45" t="s">
         <v>496</v>
-      </c>
-      <c r="C5" s="45" t="s">
-        <v>505</v>
-      </c>
-      <c r="D5" s="45" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="46" t="s">
+        <v>511</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>218</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>504</v>
+      </c>
+      <c r="D6" s="46" t="s">
         <v>204</v>
-      </c>
-      <c r="B6" s="46" t="s">
-        <v>219</v>
-      </c>
-      <c r="C6" s="46" t="s">
-        <v>505</v>
-      </c>
-      <c r="D6" s="46" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="45" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D7" s="45" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="45" t="s">
+        <v>206</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>504</v>
+      </c>
+      <c r="D8" s="45" t="s">
         <v>207</v>
-      </c>
-      <c r="B8" s="45" t="s">
-        <v>220</v>
-      </c>
-      <c r="C8" s="45" t="s">
-        <v>505</v>
-      </c>
-      <c r="D8" s="45" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="45" t="s">
+        <v>500</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>504</v>
+      </c>
+      <c r="D9" s="45" t="s">
         <v>501</v>
-      </c>
-      <c r="B9" s="45" t="s">
-        <v>220</v>
-      </c>
-      <c r="C9" s="45" t="s">
-        <v>505</v>
-      </c>
-      <c r="D9" s="45" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C10" s="46"/>
       <c r="D10" s="46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="45" t="s">
+        <v>258</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>221</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>505</v>
+      </c>
+      <c r="D11" s="45" t="s">
         <v>259</v>
-      </c>
-      <c r="B11" s="45" t="s">
-        <v>222</v>
-      </c>
-      <c r="C11" s="45" t="s">
-        <v>506</v>
-      </c>
-      <c r="D11" s="45" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C12" s="46"/>
       <c r="D12" s="46" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="45" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B13" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D13" s="45" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="45" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B14" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D14" s="45" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="45" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B15" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C15" s="45" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D15" s="45" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="45" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B16" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C16" s="45" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D16" s="45" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="45" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B17" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C17" s="45" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D17" s="45" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="46" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B18" s="46" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C18" s="46"/>
       <c r="D18" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="45" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B19" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C19" s="45" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D19" s="45" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="45" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B20" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C20" s="45" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D20" s="45" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="45" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B21" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C21" s="45" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D21" s="45" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="45" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B22" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C22" s="45" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D22" s="45" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="45" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B23" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C23" s="45" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D23" s="45" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="46" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C24" s="46"/>
       <c r="D24" s="46" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="45" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B25" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C25" s="45" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D25" s="45" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B26" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C26" s="45" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D26" s="45" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="45" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B27" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C27" s="45" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D27" s="45" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="45" t="s">
+        <v>498</v>
+      </c>
+      <c r="B28" s="45" t="s">
+        <v>221</v>
+      </c>
+      <c r="C28" s="45" t="s">
+        <v>506</v>
+      </c>
+      <c r="D28" s="45" t="s">
         <v>499</v>
-      </c>
-      <c r="B28" s="45" t="s">
-        <v>222</v>
-      </c>
-      <c r="C28" s="45" t="s">
-        <v>507</v>
-      </c>
-      <c r="D28" s="45" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B29" s="46" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C29" s="46"/>
       <c r="D29" s="46" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="45" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B30" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C30" s="45" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D30" s="45" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="45" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B31" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C31" s="45" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D31" s="45" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="45" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B32" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C32" s="45" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D32" s="45" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="45" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B33" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C33" s="45" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D33" s="45" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="45" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B34" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C34" s="45" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D34" s="45" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>